<commit_message>
custom excel + amélioration
</commit_message>
<xml_diff>
--- a/public/excel/custom.xlsx
+++ b/public/excel/custom.xlsx
@@ -434,6 +434,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="4.855957" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="12.854004" bestFit="true" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">

</xml_diff>